<commit_message>
Need to make T a collection or enumerable in MinMax report...
</commit_message>
<xml_diff>
--- a/FlatFile.UnitTests/InputFiles/GenerateTestData.xlsx
+++ b/FlatFile.UnitTests/InputFiles/GenerateTestData.xlsx
@@ -1,22 +1,132 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975771E8-B755-443E-8A0E-D38B7BBF7755}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886C2FAC-A1FC-4561-9504-E1B45C2AB4B5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NoColumnHeaders" sheetId="1" r:id="rId1"/>
+    <sheet name="Scores" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Pts</t>
+  </si>
+  <si>
+    <t>Arsenal</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>Manchester_U</t>
+  </si>
+  <si>
+    <t>Newcastle</t>
+  </si>
+  <si>
+    <t>Leeds</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>West_Ham</t>
+  </si>
+  <si>
+    <t>Aston_Villa</t>
+  </si>
+  <si>
+    <t>Tottenham</t>
+  </si>
+  <si>
+    <t>Blackburn</t>
+  </si>
+  <si>
+    <t>Southampton</t>
+  </si>
+  <si>
+    <t>Middlesbrough</t>
+  </si>
+  <si>
+    <t>Fulham</t>
+  </si>
+  <si>
+    <t>Charlton</t>
+  </si>
+  <si>
+    <t>Everton</t>
+  </si>
+  <si>
+    <t>Bolton</t>
+  </si>
+  <si>
+    <t>Sunderland</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>-----------------</t>
+  </si>
+  <si>
+    <t>-----</t>
+  </si>
+  <si>
+    <t>----</t>
+  </si>
+  <si>
+    <t>Ipswich</t>
+  </si>
+  <si>
+    <t>Derby</t>
+  </si>
+  <si>
+    <t>Leicester</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -334,16 +444,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M250"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="13" width="15.7109375" customWidth="1"/>
+    <col min="1" max="13" width="15.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1">
         <v>1</v>
       </c>
@@ -396,7 +506,7 @@
         <v>Row1Field12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>2</v>
       </c>
@@ -449,7 +559,7 @@
         <v>Row2Field12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>3</v>
       </c>
@@ -502,7 +612,7 @@
         <v>Row3Field12</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>4</v>
       </c>
@@ -555,7 +665,7 @@
         <v>Row4Field12</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>5</v>
       </c>
@@ -608,7 +718,7 @@
         <v>Row5Field12</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>6</v>
       </c>
@@ -661,7 +771,7 @@
         <v>Row6Field12</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>7</v>
       </c>
@@ -714,7 +824,7 @@
         <v>Row7Field12</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>8</v>
       </c>
@@ -767,7 +877,7 @@
         <v>Row8Field12</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>9</v>
       </c>
@@ -820,7 +930,7 @@
         <v>Row9Field12</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>10</v>
       </c>
@@ -873,7 +983,7 @@
         <v>Row10Field12</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>11</v>
       </c>
@@ -926,7 +1036,7 @@
         <v>Row11Field12</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>12</v>
       </c>
@@ -979,7 +1089,7 @@
         <v>Row12Field12</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>13</v>
       </c>
@@ -1032,7 +1142,7 @@
         <v>Row13Field12</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>14</v>
       </c>
@@ -1085,7 +1195,7 @@
         <v>Row14Field12</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>15</v>
       </c>
@@ -1138,7 +1248,7 @@
         <v>Row15Field12</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>16</v>
       </c>
@@ -1191,7 +1301,7 @@
         <v>Row16Field12</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>17</v>
       </c>
@@ -1244,7 +1354,7 @@
         <v>Row17Field12</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>18</v>
       </c>
@@ -1297,7 +1407,7 @@
         <v>Row18Field12</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>19</v>
       </c>
@@ -1350,7 +1460,7 @@
         <v>Row19Field12</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1403,7 +1513,7 @@
         <v>Row20Field12</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>21</v>
       </c>
@@ -1456,7 +1566,7 @@
         <v>Row21Field12</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>22</v>
       </c>
@@ -1509,7 +1619,7 @@
         <v>Row22Field12</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>23</v>
       </c>
@@ -1562,7 +1672,7 @@
         <v>Row23Field12</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>24</v>
       </c>
@@ -1615,7 +1725,7 @@
         <v>Row24Field12</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>25</v>
       </c>
@@ -1668,7 +1778,7 @@
         <v>Row25Field12</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>26</v>
       </c>
@@ -1721,7 +1831,7 @@
         <v>Row26Field12</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>27</v>
       </c>
@@ -1774,7 +1884,7 @@
         <v>Row27Field12</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>28</v>
       </c>
@@ -1827,7 +1937,7 @@
         <v>Row28Field12</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>29</v>
       </c>
@@ -1880,7 +1990,7 @@
         <v>Row29Field12</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>30</v>
       </c>
@@ -1933,7 +2043,7 @@
         <v>Row30Field12</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>31</v>
       </c>
@@ -1986,7 +2096,7 @@
         <v>Row31Field12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>32</v>
       </c>
@@ -2039,7 +2149,7 @@
         <v>Row32Field12</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>33</v>
       </c>
@@ -2092,7 +2202,7 @@
         <v>Row33Field12</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>34</v>
       </c>
@@ -2145,7 +2255,7 @@
         <v>Row34Field12</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>35</v>
       </c>
@@ -2198,7 +2308,7 @@
         <v>Row35Field12</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>36</v>
       </c>
@@ -2251,7 +2361,7 @@
         <v>Row36Field12</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>37</v>
       </c>
@@ -2304,7 +2414,7 @@
         <v>Row37Field12</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>38</v>
       </c>
@@ -2357,7 +2467,7 @@
         <v>Row38Field12</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>39</v>
       </c>
@@ -2410,7 +2520,7 @@
         <v>Row39Field12</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>40</v>
       </c>
@@ -2463,7 +2573,7 @@
         <v>Row40Field12</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>41</v>
       </c>
@@ -2516,7 +2626,7 @@
         <v>Row41Field12</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>42</v>
       </c>
@@ -2569,7 +2679,7 @@
         <v>Row42Field12</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>43</v>
       </c>
@@ -2622,7 +2732,7 @@
         <v>Row43Field12</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>44</v>
       </c>
@@ -2675,7 +2785,7 @@
         <v>Row44Field12</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>45</v>
       </c>
@@ -2728,7 +2838,7 @@
         <v>Row45Field12</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>46</v>
       </c>
@@ -2781,7 +2891,7 @@
         <v>Row46Field12</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>47</v>
       </c>
@@ -2834,7 +2944,7 @@
         <v>Row47Field12</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>48</v>
       </c>
@@ -2887,7 +2997,7 @@
         <v>Row48Field12</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>49</v>
       </c>
@@ -2940,7 +3050,7 @@
         <v>Row49Field12</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>50</v>
       </c>
@@ -2993,7 +3103,7 @@
         <v>Row50Field12</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>51</v>
       </c>
@@ -3046,7 +3156,7 @@
         <v>Row51Field12</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>52</v>
       </c>
@@ -3099,7 +3209,7 @@
         <v>Row52Field12</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>53</v>
       </c>
@@ -3152,7 +3262,7 @@
         <v>Row53Field12</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>54</v>
       </c>
@@ -3205,7 +3315,7 @@
         <v>Row54Field12</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>55</v>
       </c>
@@ -3258,7 +3368,7 @@
         <v>Row55Field12</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>56</v>
       </c>
@@ -3311,7 +3421,7 @@
         <v>Row56Field12</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>57</v>
       </c>
@@ -3364,7 +3474,7 @@
         <v>Row57Field12</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>58</v>
       </c>
@@ -3417,7 +3527,7 @@
         <v>Row58Field12</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>59</v>
       </c>
@@ -3470,7 +3580,7 @@
         <v>Row59Field12</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>60</v>
       </c>
@@ -3523,7 +3633,7 @@
         <v>Row60Field12</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>61</v>
       </c>
@@ -3576,7 +3686,7 @@
         <v>Row61Field12</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>62</v>
       </c>
@@ -3629,7 +3739,7 @@
         <v>Row62Field12</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>63</v>
       </c>
@@ -3682,7 +3792,7 @@
         <v>Row63Field12</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>64</v>
       </c>
@@ -3735,7 +3845,7 @@
         <v>Row64Field12</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>65</v>
       </c>
@@ -3788,7 +3898,7 @@
         <v>Row65Field12</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>66</v>
       </c>
@@ -3841,7 +3951,7 @@
         <v>Row66Field12</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>67</v>
       </c>
@@ -3894,7 +4004,7 @@
         <v>Row67Field12</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>68</v>
       </c>
@@ -3947,7 +4057,7 @@
         <v>Row68Field12</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>69</v>
       </c>
@@ -4000,7 +4110,7 @@
         <v>Row69Field12</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>70</v>
       </c>
@@ -4053,7 +4163,7 @@
         <v>Row70Field12</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>71</v>
       </c>
@@ -4106,7 +4216,7 @@
         <v>Row71Field12</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>72</v>
       </c>
@@ -4159,7 +4269,7 @@
         <v>Row72Field12</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>73</v>
       </c>
@@ -4212,7 +4322,7 @@
         <v>Row73Field12</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>74</v>
       </c>
@@ -4265,7 +4375,7 @@
         <v>Row74Field12</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>75</v>
       </c>
@@ -4318,7 +4428,7 @@
         <v>Row75Field12</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>76</v>
       </c>
@@ -4371,7 +4481,7 @@
         <v>Row76Field12</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>77</v>
       </c>
@@ -4424,7 +4534,7 @@
         <v>Row77Field12</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>78</v>
       </c>
@@ -4477,7 +4587,7 @@
         <v>Row78Field12</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>79</v>
       </c>
@@ -4530,7 +4640,7 @@
         <v>Row79Field12</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>80</v>
       </c>
@@ -4583,7 +4693,7 @@
         <v>Row80Field12</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>81</v>
       </c>
@@ -4636,7 +4746,7 @@
         <v>Row81Field12</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>82</v>
       </c>
@@ -4689,7 +4799,7 @@
         <v>Row82Field12</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>83</v>
       </c>
@@ -4742,7 +4852,7 @@
         <v>Row83Field12</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>84</v>
       </c>
@@ -4795,7 +4905,7 @@
         <v>Row84Field12</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>85</v>
       </c>
@@ -4848,7 +4958,7 @@
         <v>Row85Field12</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>86</v>
       </c>
@@ -4901,7 +5011,7 @@
         <v>Row86Field12</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>87</v>
       </c>
@@ -4954,7 +5064,7 @@
         <v>Row87Field12</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>88</v>
       </c>
@@ -5007,7 +5117,7 @@
         <v>Row88Field12</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>89</v>
       </c>
@@ -5060,7 +5170,7 @@
         <v>Row89Field12</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>90</v>
       </c>
@@ -5113,7 +5223,7 @@
         <v>Row90Field12</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>91</v>
       </c>
@@ -5166,7 +5276,7 @@
         <v>Row91Field12</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>92</v>
       </c>
@@ -5219,7 +5329,7 @@
         <v>Row92Field12</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>93</v>
       </c>
@@ -5272,7 +5382,7 @@
         <v>Row93Field12</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A94">
         <v>94</v>
       </c>
@@ -5325,7 +5435,7 @@
         <v>Row94Field12</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A95">
         <v>95</v>
       </c>
@@ -5378,7 +5488,7 @@
         <v>Row95Field12</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A96">
         <v>96</v>
       </c>
@@ -5431,7 +5541,7 @@
         <v>Row96Field12</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A97">
         <v>97</v>
       </c>
@@ -5484,7 +5594,7 @@
         <v>Row97Field12</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A98">
         <v>98</v>
       </c>
@@ -5537,7 +5647,7 @@
         <v>Row98Field12</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A99">
         <v>99</v>
       </c>
@@ -5590,7 +5700,7 @@
         <v>Row99Field12</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A100">
         <v>100</v>
       </c>
@@ -5643,7 +5753,7 @@
         <v>Row100Field12</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A101">
         <v>101</v>
       </c>
@@ -5696,7 +5806,7 @@
         <v>Row101Field12</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A102">
         <v>102</v>
       </c>
@@ -5749,7 +5859,7 @@
         <v>Row102Field12</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A103">
         <v>103</v>
       </c>
@@ -5802,7 +5912,7 @@
         <v>Row103Field12</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A104">
         <v>104</v>
       </c>
@@ -5855,7 +5965,7 @@
         <v>Row104Field12</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A105">
         <v>105</v>
       </c>
@@ -5908,7 +6018,7 @@
         <v>Row105Field12</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A106">
         <v>106</v>
       </c>
@@ -5961,7 +6071,7 @@
         <v>Row106Field12</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A107">
         <v>107</v>
       </c>
@@ -6014,7 +6124,7 @@
         <v>Row107Field12</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A108">
         <v>108</v>
       </c>
@@ -6067,7 +6177,7 @@
         <v>Row108Field12</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A109">
         <v>109</v>
       </c>
@@ -6120,7 +6230,7 @@
         <v>Row109Field12</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A110">
         <v>110</v>
       </c>
@@ -6173,7 +6283,7 @@
         <v>Row110Field12</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A111">
         <v>111</v>
       </c>
@@ -6226,7 +6336,7 @@
         <v>Row111Field12</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A112">
         <v>112</v>
       </c>
@@ -6279,7 +6389,7 @@
         <v>Row112Field12</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A113">
         <v>113</v>
       </c>
@@ -6332,7 +6442,7 @@
         <v>Row113Field12</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A114">
         <v>114</v>
       </c>
@@ -6385,7 +6495,7 @@
         <v>Row114Field12</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A115">
         <v>115</v>
       </c>
@@ -6438,7 +6548,7 @@
         <v>Row115Field12</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A116">
         <v>116</v>
       </c>
@@ -6491,7 +6601,7 @@
         <v>Row116Field12</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A117">
         <v>117</v>
       </c>
@@ -6544,7 +6654,7 @@
         <v>Row117Field12</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A118">
         <v>118</v>
       </c>
@@ -6597,7 +6707,7 @@
         <v>Row118Field12</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A119">
         <v>119</v>
       </c>
@@ -6650,7 +6760,7 @@
         <v>Row119Field12</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A120">
         <v>120</v>
       </c>
@@ -6703,7 +6813,7 @@
         <v>Row120Field12</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A121">
         <v>121</v>
       </c>
@@ -6756,7 +6866,7 @@
         <v>Row121Field12</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A122">
         <v>122</v>
       </c>
@@ -6809,7 +6919,7 @@
         <v>Row122Field12</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A123">
         <v>123</v>
       </c>
@@ -6862,7 +6972,7 @@
         <v>Row123Field12</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A124">
         <v>124</v>
       </c>
@@ -6915,7 +7025,7 @@
         <v>Row124Field12</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A125">
         <v>125</v>
       </c>
@@ -6968,7 +7078,7 @@
         <v>Row125Field12</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A126">
         <v>126</v>
       </c>
@@ -7021,7 +7131,7 @@
         <v>Row126Field12</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A127">
         <v>127</v>
       </c>
@@ -7074,7 +7184,7 @@
         <v>Row127Field12</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A128">
         <v>128</v>
       </c>
@@ -7127,7 +7237,7 @@
         <v>Row128Field12</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A129">
         <v>129</v>
       </c>
@@ -7180,7 +7290,7 @@
         <v>Row129Field12</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A130">
         <v>130</v>
       </c>
@@ -7233,7 +7343,7 @@
         <v>Row130Field12</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A131">
         <v>131</v>
       </c>
@@ -7286,7 +7396,7 @@
         <v>Row131Field12</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A132">
         <v>132</v>
       </c>
@@ -7339,7 +7449,7 @@
         <v>Row132Field12</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A133">
         <v>133</v>
       </c>
@@ -7392,7 +7502,7 @@
         <v>Row133Field12</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A134">
         <v>134</v>
       </c>
@@ -7445,7 +7555,7 @@
         <v>Row134Field12</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A135">
         <v>135</v>
       </c>
@@ -7498,7 +7608,7 @@
         <v>Row135Field12</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A136">
         <v>136</v>
       </c>
@@ -7551,7 +7661,7 @@
         <v>Row136Field12</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A137">
         <v>137</v>
       </c>
@@ -7604,7 +7714,7 @@
         <v>Row137Field12</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A138">
         <v>138</v>
       </c>
@@ -7657,7 +7767,7 @@
         <v>Row138Field12</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A139">
         <v>139</v>
       </c>
@@ -7710,7 +7820,7 @@
         <v>Row139Field12</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A140">
         <v>140</v>
       </c>
@@ -7763,7 +7873,7 @@
         <v>Row140Field12</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A141">
         <v>141</v>
       </c>
@@ -7816,7 +7926,7 @@
         <v>Row141Field12</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A142">
         <v>142</v>
       </c>
@@ -7869,7 +7979,7 @@
         <v>Row142Field12</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A143">
         <v>143</v>
       </c>
@@ -7922,7 +8032,7 @@
         <v>Row143Field12</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A144">
         <v>144</v>
       </c>
@@ -7975,7 +8085,7 @@
         <v>Row144Field12</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A145">
         <v>145</v>
       </c>
@@ -8028,7 +8138,7 @@
         <v>Row145Field12</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A146">
         <v>146</v>
       </c>
@@ -8081,7 +8191,7 @@
         <v>Row146Field12</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A147">
         <v>147</v>
       </c>
@@ -8134,7 +8244,7 @@
         <v>Row147Field12</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A148">
         <v>148</v>
       </c>
@@ -8187,7 +8297,7 @@
         <v>Row148Field12</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A149">
         <v>149</v>
       </c>
@@ -8240,7 +8350,7 @@
         <v>Row149Field12</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A150">
         <v>150</v>
       </c>
@@ -8293,7 +8403,7 @@
         <v>Row150Field12</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A151">
         <v>151</v>
       </c>
@@ -8346,7 +8456,7 @@
         <v>Row151Field12</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A152">
         <v>152</v>
       </c>
@@ -8399,7 +8509,7 @@
         <v>Row152Field12</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A153">
         <v>153</v>
       </c>
@@ -8452,7 +8562,7 @@
         <v>Row153Field12</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A154">
         <v>154</v>
       </c>
@@ -8505,7 +8615,7 @@
         <v>Row154Field12</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A155">
         <v>155</v>
       </c>
@@ -8558,7 +8668,7 @@
         <v>Row155Field12</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A156">
         <v>156</v>
       </c>
@@ -8611,7 +8721,7 @@
         <v>Row156Field12</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A157">
         <v>157</v>
       </c>
@@ -8664,7 +8774,7 @@
         <v>Row157Field12</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A158">
         <v>158</v>
       </c>
@@ -8717,7 +8827,7 @@
         <v>Row158Field12</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A159">
         <v>159</v>
       </c>
@@ -8770,7 +8880,7 @@
         <v>Row159Field12</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A160">
         <v>160</v>
       </c>
@@ -8823,7 +8933,7 @@
         <v>Row160Field12</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A161">
         <v>161</v>
       </c>
@@ -8876,7 +8986,7 @@
         <v>Row161Field12</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A162">
         <v>162</v>
       </c>
@@ -8929,7 +9039,7 @@
         <v>Row162Field12</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A163">
         <v>163</v>
       </c>
@@ -8982,7 +9092,7 @@
         <v>Row163Field12</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A164">
         <v>164</v>
       </c>
@@ -9035,7 +9145,7 @@
         <v>Row164Field12</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A165">
         <v>165</v>
       </c>
@@ -9088,7 +9198,7 @@
         <v>Row165Field12</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A166">
         <v>166</v>
       </c>
@@ -9141,7 +9251,7 @@
         <v>Row166Field12</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A167">
         <v>167</v>
       </c>
@@ -9194,7 +9304,7 @@
         <v>Row167Field12</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A168">
         <v>168</v>
       </c>
@@ -9247,7 +9357,7 @@
         <v>Row168Field12</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A169">
         <v>169</v>
       </c>
@@ -9300,7 +9410,7 @@
         <v>Row169Field12</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A170">
         <v>170</v>
       </c>
@@ -9353,7 +9463,7 @@
         <v>Row170Field12</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A171">
         <v>171</v>
       </c>
@@ -9406,7 +9516,7 @@
         <v>Row171Field12</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A172">
         <v>172</v>
       </c>
@@ -9459,7 +9569,7 @@
         <v>Row172Field12</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A173">
         <v>173</v>
       </c>
@@ -9512,7 +9622,7 @@
         <v>Row173Field12</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A174">
         <v>174</v>
       </c>
@@ -9565,7 +9675,7 @@
         <v>Row174Field12</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A175">
         <v>175</v>
       </c>
@@ -9618,7 +9728,7 @@
         <v>Row175Field12</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A176">
         <v>176</v>
       </c>
@@ -9671,7 +9781,7 @@
         <v>Row176Field12</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A177">
         <v>177</v>
       </c>
@@ -9724,7 +9834,7 @@
         <v>Row177Field12</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A178">
         <v>178</v>
       </c>
@@ -9777,7 +9887,7 @@
         <v>Row178Field12</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A179">
         <v>179</v>
       </c>
@@ -9830,7 +9940,7 @@
         <v>Row179Field12</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A180">
         <v>180</v>
       </c>
@@ -9883,7 +9993,7 @@
         <v>Row180Field12</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A181">
         <v>181</v>
       </c>
@@ -9936,7 +10046,7 @@
         <v>Row181Field12</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A182">
         <v>182</v>
       </c>
@@ -9989,7 +10099,7 @@
         <v>Row182Field12</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A183">
         <v>183</v>
       </c>
@@ -10042,7 +10152,7 @@
         <v>Row183Field12</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A184">
         <v>184</v>
       </c>
@@ -10095,7 +10205,7 @@
         <v>Row184Field12</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A185">
         <v>185</v>
       </c>
@@ -10148,7 +10258,7 @@
         <v>Row185Field12</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A186">
         <v>186</v>
       </c>
@@ -10201,7 +10311,7 @@
         <v>Row186Field12</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A187">
         <v>187</v>
       </c>
@@ -10254,7 +10364,7 @@
         <v>Row187Field12</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A188">
         <v>188</v>
       </c>
@@ -10307,7 +10417,7 @@
         <v>Row188Field12</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A189">
         <v>189</v>
       </c>
@@ -10360,7 +10470,7 @@
         <v>Row189Field12</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A190">
         <v>190</v>
       </c>
@@ -10413,7 +10523,7 @@
         <v>Row190Field12</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A191">
         <v>191</v>
       </c>
@@ -10466,7 +10576,7 @@
         <v>Row191Field12</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A192">
         <v>192</v>
       </c>
@@ -10519,7 +10629,7 @@
         <v>Row192Field12</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A193">
         <v>193</v>
       </c>
@@ -10572,7 +10682,7 @@
         <v>Row193Field12</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A194">
         <v>194</v>
       </c>
@@ -10625,7 +10735,7 @@
         <v>Row194Field12</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A195">
         <v>195</v>
       </c>
@@ -10678,7 +10788,7 @@
         <v>Row195Field12</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A196">
         <v>196</v>
       </c>
@@ -10731,7 +10841,7 @@
         <v>Row196Field12</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A197">
         <v>197</v>
       </c>
@@ -10784,7 +10894,7 @@
         <v>Row197Field12</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A198">
         <v>198</v>
       </c>
@@ -10837,7 +10947,7 @@
         <v>Row198Field12</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A199">
         <v>199</v>
       </c>
@@ -10890,7 +11000,7 @@
         <v>Row199Field12</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A200">
         <v>200</v>
       </c>
@@ -10943,7 +11053,7 @@
         <v>Row200Field12</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A201">
         <v>201</v>
       </c>
@@ -10996,7 +11106,7 @@
         <v>Row201Field12</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A202">
         <v>202</v>
       </c>
@@ -11049,7 +11159,7 @@
         <v>Row202Field12</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A203">
         <v>203</v>
       </c>
@@ -11102,7 +11212,7 @@
         <v>Row203Field12</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A204">
         <v>204</v>
       </c>
@@ -11155,7 +11265,7 @@
         <v>Row204Field12</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A205">
         <v>205</v>
       </c>
@@ -11208,7 +11318,7 @@
         <v>Row205Field12</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A206">
         <v>206</v>
       </c>
@@ -11261,7 +11371,7 @@
         <v>Row206Field12</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A207">
         <v>207</v>
       </c>
@@ -11314,7 +11424,7 @@
         <v>Row207Field12</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A208">
         <v>208</v>
       </c>
@@ -11367,7 +11477,7 @@
         <v>Row208Field12</v>
       </c>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A209">
         <v>209</v>
       </c>
@@ -11420,7 +11530,7 @@
         <v>Row209Field12</v>
       </c>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A210">
         <v>210</v>
       </c>
@@ -11473,7 +11583,7 @@
         <v>Row210Field12</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A211">
         <v>211</v>
       </c>
@@ -11526,7 +11636,7 @@
         <v>Row211Field12</v>
       </c>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A212">
         <v>212</v>
       </c>
@@ -11579,7 +11689,7 @@
         <v>Row212Field12</v>
       </c>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A213">
         <v>213</v>
       </c>
@@ -11632,7 +11742,7 @@
         <v>Row213Field12</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A214">
         <v>214</v>
       </c>
@@ -11685,7 +11795,7 @@
         <v>Row214Field12</v>
       </c>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A215">
         <v>215</v>
       </c>
@@ -11738,7 +11848,7 @@
         <v>Row215Field12</v>
       </c>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A216">
         <v>216</v>
       </c>
@@ -11791,7 +11901,7 @@
         <v>Row216Field12</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A217">
         <v>217</v>
       </c>
@@ -11844,7 +11954,7 @@
         <v>Row217Field12</v>
       </c>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A218">
         <v>218</v>
       </c>
@@ -11897,7 +12007,7 @@
         <v>Row218Field12</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A219">
         <v>219</v>
       </c>
@@ -11950,7 +12060,7 @@
         <v>Row219Field12</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A220">
         <v>220</v>
       </c>
@@ -12003,7 +12113,7 @@
         <v>Row220Field12</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A221">
         <v>221</v>
       </c>
@@ -12056,7 +12166,7 @@
         <v>Row221Field12</v>
       </c>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A222">
         <v>222</v>
       </c>
@@ -12109,7 +12219,7 @@
         <v>Row222Field12</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A223">
         <v>223</v>
       </c>
@@ -12162,7 +12272,7 @@
         <v>Row223Field12</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A224">
         <v>224</v>
       </c>
@@ -12215,7 +12325,7 @@
         <v>Row224Field12</v>
       </c>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A225">
         <v>225</v>
       </c>
@@ -12268,7 +12378,7 @@
         <v>Row225Field12</v>
       </c>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A226">
         <v>226</v>
       </c>
@@ -12321,7 +12431,7 @@
         <v>Row226Field12</v>
       </c>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A227">
         <v>227</v>
       </c>
@@ -12374,7 +12484,7 @@
         <v>Row227Field12</v>
       </c>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A228">
         <v>228</v>
       </c>
@@ -12427,7 +12537,7 @@
         <v>Row228Field12</v>
       </c>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A229">
         <v>229</v>
       </c>
@@ -12480,7 +12590,7 @@
         <v>Row229Field12</v>
       </c>
     </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A230">
         <v>230</v>
       </c>
@@ -12533,7 +12643,7 @@
         <v>Row230Field12</v>
       </c>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A231">
         <v>231</v>
       </c>
@@ -12586,7 +12696,7 @@
         <v>Row231Field12</v>
       </c>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A232">
         <v>232</v>
       </c>
@@ -12639,7 +12749,7 @@
         <v>Row232Field12</v>
       </c>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A233">
         <v>233</v>
       </c>
@@ -12692,7 +12802,7 @@
         <v>Row233Field12</v>
       </c>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A234">
         <v>234</v>
       </c>
@@ -12745,7 +12855,7 @@
         <v>Row234Field12</v>
       </c>
     </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A235">
         <v>235</v>
       </c>
@@ -12798,7 +12908,7 @@
         <v>Row235Field12</v>
       </c>
     </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A236">
         <v>236</v>
       </c>
@@ -12851,7 +12961,7 @@
         <v>Row236Field12</v>
       </c>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A237">
         <v>237</v>
       </c>
@@ -12904,7 +13014,7 @@
         <v>Row237Field12</v>
       </c>
     </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A238">
         <v>238</v>
       </c>
@@ -12957,7 +13067,7 @@
         <v>Row238Field12</v>
       </c>
     </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A239">
         <v>239</v>
       </c>
@@ -13010,7 +13120,7 @@
         <v>Row239Field12</v>
       </c>
     </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A240">
         <v>240</v>
       </c>
@@ -13063,7 +13173,7 @@
         <v>Row240Field12</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A241">
         <v>241</v>
       </c>
@@ -13116,7 +13226,7 @@
         <v>Row241Field12</v>
       </c>
     </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A242">
         <v>242</v>
       </c>
@@ -13169,7 +13279,7 @@
         <v>Row242Field12</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A243">
         <v>243</v>
       </c>
@@ -13222,7 +13332,7 @@
         <v>Row243Field12</v>
       </c>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A244">
         <v>244</v>
       </c>
@@ -13275,7 +13385,7 @@
         <v>Row244Field12</v>
       </c>
     </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A245">
         <v>245</v>
       </c>
@@ -13328,7 +13438,7 @@
         <v>Row245Field12</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A246">
         <v>246</v>
       </c>
@@ -13381,7 +13491,7 @@
         <v>Row246Field12</v>
       </c>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A247">
         <v>247</v>
       </c>
@@ -13434,7 +13544,7 @@
         <v>Row247Field12</v>
       </c>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A248">
         <v>248</v>
       </c>
@@ -13487,7 +13597,7 @@
         <v>Row248Field12</v>
       </c>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A249">
         <v>249</v>
       </c>
@@ -13540,7 +13650,7 @@
         <v>Row249Field12</v>
       </c>
     </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A250">
         <v>250</v>
       </c>
@@ -13596,4 +13706,886 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F9CA70-2F18-44B5-BBD4-69E01F79D1A7}">
+  <dimension ref="A1:O22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>38</v>
+      </c>
+      <c r="D2">
+        <v>26</v>
+      </c>
+      <c r="E2">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>79</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2">
+        <v>36</v>
+      </c>
+      <c r="J2">
+        <v>87</v>
+      </c>
+      <c r="M2" t="str">
+        <f>"""" &amp; B2 &amp; """, " &amp; G2 &amp; ", " &amp; I2</f>
+        <v>"Arsenal", 79, 36</v>
+      </c>
+      <c r="O2" t="str">
+        <f>"new LeagueScore(" &amp; M2 &amp; "),"</f>
+        <v>new LeagueScore("Arsenal", 79, 36),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>38</v>
+      </c>
+      <c r="D3">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>67</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <v>30</v>
+      </c>
+      <c r="J3">
+        <v>80</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" ref="M3:M22" si="0">"""" &amp; B3 &amp; """, " &amp; G3 &amp; ", " &amp; I3</f>
+        <v>"Liverpool", 67, 30</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O22" si="1">"new LeagueScore(" &amp; M3 &amp; "),"</f>
+        <v>new LeagueScore("Liverpool", 67, 30),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>38</v>
+      </c>
+      <c r="D4">
+        <v>24</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>87</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4">
+        <v>45</v>
+      </c>
+      <c r="J4">
+        <v>77</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="0"/>
+        <v>"Manchester_U", 87, 45</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("Manchester_U", 87, 45),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>38</v>
+      </c>
+      <c r="D5">
+        <v>21</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>74</v>
+      </c>
+      <c r="H5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5">
+        <v>52</v>
+      </c>
+      <c r="J5">
+        <v>71</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="0"/>
+        <v>"Newcastle", 74, 52</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("Newcastle", 74, 52),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>38</v>
+      </c>
+      <c r="D6">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>53</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6">
+        <v>37</v>
+      </c>
+      <c r="J6">
+        <v>66</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="0"/>
+        <v>"Leeds", 53, 37</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("Leeds", 53, 37),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>38</v>
+      </c>
+      <c r="D7">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>13</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>66</v>
+      </c>
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7">
+        <v>38</v>
+      </c>
+      <c r="J7">
+        <v>64</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" si="0"/>
+        <v>"Chelsea", 66, 38</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("Chelsea", 66, 38),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>38</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>15</v>
+      </c>
+      <c r="G8">
+        <v>48</v>
+      </c>
+      <c r="H8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8">
+        <v>57</v>
+      </c>
+      <c r="J8">
+        <v>53</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" si="0"/>
+        <v>"West_Ham", 48, 57</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("West_Ham", 48, 57),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>38</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="E9">
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <v>12</v>
+      </c>
+      <c r="G9">
+        <v>46</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9">
+        <v>47</v>
+      </c>
+      <c r="J9">
+        <v>50</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" si="0"/>
+        <v>"Aston_Villa", 46, 47</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("Aston_Villa", 46, 47),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>38</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>16</v>
+      </c>
+      <c r="G10">
+        <v>49</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10">
+        <v>53</v>
+      </c>
+      <c r="J10">
+        <v>50</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" si="0"/>
+        <v>"Tottenham", 49, 53</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("Tottenham", 49, 53),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>38</v>
+      </c>
+      <c r="D11">
+        <v>12</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>16</v>
+      </c>
+      <c r="G11">
+        <v>55</v>
+      </c>
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11">
+        <v>51</v>
+      </c>
+      <c r="J11">
+        <v>46</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" si="0"/>
+        <v>"Blackburn", 55, 51</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("Blackburn", 55, 51),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>38</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <v>17</v>
+      </c>
+      <c r="G12">
+        <v>46</v>
+      </c>
+      <c r="H12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12">
+        <v>54</v>
+      </c>
+      <c r="J12">
+        <v>45</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" si="0"/>
+        <v>"Southampton", 46, 54</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("Southampton", 46, 54),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>38</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13">
+        <v>9</v>
+      </c>
+      <c r="F13">
+        <v>17</v>
+      </c>
+      <c r="G13">
+        <v>35</v>
+      </c>
+      <c r="H13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13">
+        <v>47</v>
+      </c>
+      <c r="J13">
+        <v>45</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="0"/>
+        <v>"Middlesbrough", 35, 47</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("Middlesbrough", 35, 47),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>38</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>14</v>
+      </c>
+      <c r="F14">
+        <v>14</v>
+      </c>
+      <c r="G14">
+        <v>36</v>
+      </c>
+      <c r="H14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14">
+        <v>44</v>
+      </c>
+      <c r="J14">
+        <v>44</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" si="0"/>
+        <v>"Fulham", 36, 44</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("Fulham", 36, 44),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>38</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+      <c r="E15">
+        <v>14</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>38</v>
+      </c>
+      <c r="H15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15">
+        <v>49</v>
+      </c>
+      <c r="J15">
+        <v>44</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" si="0"/>
+        <v>"Charlton", 38, 49</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("Charlton", 38, 49),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>38</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>17</v>
+      </c>
+      <c r="G16">
+        <v>45</v>
+      </c>
+      <c r="H16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16">
+        <v>57</v>
+      </c>
+      <c r="J16">
+        <v>43</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" si="0"/>
+        <v>"Everton", 45, 57</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("Everton", 45, 57),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17">
+        <v>38</v>
+      </c>
+      <c r="D17">
+        <v>9</v>
+      </c>
+      <c r="E17">
+        <v>13</v>
+      </c>
+      <c r="F17">
+        <v>16</v>
+      </c>
+      <c r="G17">
+        <v>44</v>
+      </c>
+      <c r="H17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17">
+        <v>62</v>
+      </c>
+      <c r="J17">
+        <v>40</v>
+      </c>
+      <c r="M17" t="str">
+        <f t="shared" si="0"/>
+        <v>"Bolton", 44, 62</v>
+      </c>
+      <c r="O17" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("Bolton", 44, 62),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="F18">
+        <v>18</v>
+      </c>
+      <c r="G18">
+        <v>29</v>
+      </c>
+      <c r="H18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18">
+        <v>51</v>
+      </c>
+      <c r="J18">
+        <v>40</v>
+      </c>
+      <c r="M18" t="str">
+        <f t="shared" si="0"/>
+        <v>"Sunderland", 29, 51</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("Sunderland", 29, 51),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" t="s">
+        <v>26</v>
+      </c>
+      <c r="I19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" t="s">
+        <v>28</v>
+      </c>
+      <c r="M19" t="str">
+        <f t="shared" si="0"/>
+        <v>"-----------------", -----, -----</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("-----------------", -----, -----),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20">
+        <v>38</v>
+      </c>
+      <c r="D20">
+        <v>9</v>
+      </c>
+      <c r="E20">
+        <v>9</v>
+      </c>
+      <c r="F20">
+        <v>20</v>
+      </c>
+      <c r="G20">
+        <v>41</v>
+      </c>
+      <c r="H20" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20">
+        <v>64</v>
+      </c>
+      <c r="J20">
+        <v>36</v>
+      </c>
+      <c r="M20" t="str">
+        <f t="shared" si="0"/>
+        <v>"Ipswich", 41, 64</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("Ipswich", 41, 64),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21">
+        <v>38</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+      <c r="E21">
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <v>24</v>
+      </c>
+      <c r="G21">
+        <v>33</v>
+      </c>
+      <c r="H21" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21">
+        <v>63</v>
+      </c>
+      <c r="J21">
+        <v>30</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" si="0"/>
+        <v>"Derby", 33, 63</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("Derby", 33, 63),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22">
+        <v>38</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>13</v>
+      </c>
+      <c r="F22">
+        <v>20</v>
+      </c>
+      <c r="G22">
+        <v>30</v>
+      </c>
+      <c r="H22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22">
+        <v>64</v>
+      </c>
+      <c r="J22">
+        <v>28</v>
+      </c>
+      <c r="M22" t="str">
+        <f t="shared" si="0"/>
+        <v>"Leicester", 30, 64</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="1"/>
+        <v>new LeagueScore("Leicester", 30, 64),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
 </file>
</xml_diff>